<commit_message>
Add font style and web font
</commit_message>
<xml_diff>
--- a/软三信息统计.xlsx
+++ b/软三信息统计.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -19,10 +19,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>作者</author>
+    <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="N2" authorId="0" shapeId="0">
+    <comment ref="N2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -33,7 +33,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>作者:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -223,17 +223,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -241,14 +241,14 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="24"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -271,7 +271,7 @@
       <b/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -280,7 +280,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -288,14 +288,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -494,8 +494,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="百分比" xfId="1" builtinId="5"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -511,7 +511,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -553,7 +553,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -588,7 +588,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -800,25 +800,25 @@
   <dimension ref="A1:XFD16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.25" customWidth="1"/>
-    <col min="4" max="4" width="24.375" customWidth="1"/>
-    <col min="5" max="5" width="11.875" customWidth="1"/>
-    <col min="6" max="7" width="17.25" customWidth="1"/>
-    <col min="8" max="8" width="11.875" customWidth="1"/>
-    <col min="9" max="9" width="11.5" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
     <col min="10" max="11" width="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.25" customWidth="1"/>
-    <col min="13" max="13" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.875" customWidth="1"/>
+    <col min="12" max="12" width="26.28515625" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" ht="31.5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16384" ht="31.5">
       <c r="A1" s="19" t="s">
         <v>15</v>
       </c>
@@ -838,7 +838,7 @@
       <c r="O1" s="19"/>
       <c r="P1" s="19"/>
     </row>
-    <row r="2" spans="1:16384" ht="56.25" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16384" ht="75">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -888,7 +888,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:16384" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16384" ht="20.100000000000001" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>18</v>
@@ -933,10 +933,10 @@
         <v>37</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:16384" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16384" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="5"/>
       <c r="B4" s="6" t="s">
         <v>22</v>
@@ -984,7 +984,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:16384" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16384" s="11" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
         <v>22</v>
@@ -17400,7 +17400,7 @@
       <c r="XFC5" s="9"/>
       <c r="XFD5" s="9"/>
     </row>
-    <row r="6" spans="1:16384" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16384" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="8"/>
       <c r="B6" s="2" t="s">
         <v>22</v>
@@ -17448,7 +17448,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:16384" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16384" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
         <v>22</v>
@@ -17496,7 +17496,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:16384" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16384" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -17514,7 +17514,7 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
     </row>
-    <row r="9" spans="1:16384" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16384" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -17532,7 +17532,7 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
     </row>
-    <row r="10" spans="1:16384" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16384" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -17550,7 +17550,7 @@
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
     </row>
-    <row r="11" spans="1:16384" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16384" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -17568,7 +17568,7 @@
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
     </row>
-    <row r="12" spans="1:16384" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16384" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -17586,8 +17586,8 @@
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
     </row>
-    <row r="14" spans="1:16384" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:16384" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:16384" ht="15.75" thickBot="1"/>
+    <row r="15" spans="1:16384" ht="13.5" customHeight="1">
       <c r="A15" s="13" t="s">
         <v>16</v>
       </c>
@@ -17606,7 +17606,7 @@
       <c r="N15" s="14"/>
       <c r="O15" s="15"/>
     </row>
-    <row r="16" spans="1:16384" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16384" ht="13.5" customHeight="1" thickBot="1">
       <c r="A16" s="16"/>
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>

</xml_diff>